<commit_message>
up data ilca complit
</commit_message>
<xml_diff>
--- a/scrapers/source-data/references.xlsx
+++ b/scrapers/source-data/references.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabmel\OneDrive\Documentos\fgv\field\-sailing-rankings-2024.1\scrapers\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EBFFCE-1487-474A-BDB1-525B1A9AEA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33279094-CCB6-45E1-BA0B-DBE4D944E257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="139">
   <si>
     <t>Classe Vela</t>
   </si>
@@ -243,38 +243,212 @@
     <t>https://manage2sail.com/api/event/be360bf4-0c4b-459c-afd1-6b87d2810950/regattaresult/894c9877-ae69-4de9-824c-b88dbe6c6498</t>
   </si>
   <si>
-    <t>Eesti Meistrivõistlused 2023</t>
-  </si>
-  <si>
-    <t>https://manage2sail.com/api/event/58e7b02f-4d6a-4310-9206-d7eb493fedac/regattaresult/49er</t>
-  </si>
-  <si>
-    <t>IDM / IDJoM 2023</t>
-  </si>
-  <si>
-    <t>40erFX</t>
-  </si>
-  <si>
-    <t>https://manage2sail.com/api/event/e4af1af6-1b2f-42b9-89a8-8e3664301c41/regattaresult/JoM49</t>
-  </si>
-  <si>
-    <t>https://manage2sail.com/api/event/e4af1af6-1b2f-42b9-89a8-8e3664301c41/regattaresult/JoMFX</t>
-  </si>
-  <si>
     <t>Esquife DS-DM 2023</t>
   </si>
   <si>
-    <t>https://manage2sail.com/api/event/a799a094-bd7a-487a-a1fa-2acddaf40dbd/regattaresult/1db95acb-adcd-467a-adbe-d9143db24286</t>
-  </si>
-  <si>
     <t>https://manage2sail.com/api/event/a799a094-bd7a-487a-a1fa-2acddaf40dbd/regattaresult/4fc4dbf4-536f-4b58-86e9-6a32f49bdc49</t>
+  </si>
+  <si>
+    <t>ilca 7</t>
+  </si>
+  <si>
+    <t>ilca 6</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/92afe9f9-1611-47fb-a28c-aca4e41a589d/regattaresult/177e915a-96ac-498e-b115-b74766a63cba</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/92afe9f9-1611-47fb-a28c-aca4e41a589d/regattaresult/194d9758-9808-4c53-b41a-730741d53000</t>
+  </si>
+  <si>
+    <t>CAMPEONATO ABERTO BELGA 2023</t>
+  </si>
+  <si>
+    <t>ILCA Nacional 1 ZC Hofstade 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/5a58fee5-849c-4193-9d9e-713dac2c661d/regattaresult/f45f619b-df96-4c39-993c-3fc131b6e44b</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/5a58fee5-849c-4193-9d9e-713dac2c661d/regattaresult/e24d5e60-4387-4451-a651-3d84216b3861</t>
+  </si>
+  <si>
+    <t>Kupferne Rohrdommel - Distriktmeisterschaft Nord 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/1e8935a4-601a-4805-a3aa-97d0bf372aab/regattaresult/5ceaa952-587d-4c49-9d53-f6fb20359b37</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/1e8935a4-601a-4805-a3aa-97d0bf372aab/regattaresult/35fef37c-d106-4fb2-9488-46c2d3047f92</t>
+  </si>
+  <si>
+    <t>EURILCA MASTER SERIES BÉLGICA 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/3670ccd7-1fc8-4f2b-9db4-3179960a08a7/regattaresult/ce2de4e7-aeec-4575-8a3f-b795b41d1f48</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/3670ccd7-1fc8-4f2b-9db4-3179960a08a7/regattaresult/d6faf791-25c0-4f8f-96c5-f0b288cdb212</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/651b64e8-24a5-4095-ba77-7992789f3309/regattaresult/1a331330-8f96-44a8-8702-7aa9db70cc3f</t>
+  </si>
+  <si>
+    <t>Regata ILCA 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/589739b7-a39e-460a-baec-c6610ca96d1a/regattaresult/f6624ecf-6cfb-4431-b750-d3e2fdac40bf</t>
+  </si>
+  <si>
+    <t>Opti-Europa-ILCA Treff Bosau 2023</t>
+  </si>
+  <si>
+    <t>Norgesmesterskap ILCA e Optimist 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/670cfed9-996a-427c-922c-a6b0af34586c/regattaresult/47735c4b-670a-4368-a39b-801f8baad69f</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/670cfed9-996a-427c-922c-a6b0af34586c/regattaresult/db9a9e08-89a1-4088-891a-fe76c23cdc31</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/d4027706-2a82-41c9-a172-4e935fae8739/regattaresult/9a1759fd-a191-4f4f-8ff9-0d8aaedc9100</t>
+  </si>
+  <si>
+    <t>ILCA Punktemeisterschaft 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/12442ff0-3f37-4bff-88d4-87e8bb5a86c8/regattaresult/f8ef8dcd-7696-4d19-8fb4-afc27c4fea46</t>
+  </si>
+  <si>
+    <t>Escola laser 2023</t>
+  </si>
+  <si>
+    <t>Troféu Königswinkel ILCA 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/62fd50b1-1876-4c16-8e86-608bf7f1d06a/regattaresult/27049377-9bec-40e9-8699-6ef2b24327d0</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/62fd50b1-1876-4c16-8e86-608bf7f1d06a/regattaresult/e64b5966-d07a-47ce-b0f7-bff3af41fcd7</t>
+  </si>
+  <si>
+    <t>IDJM 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/8c0efde4-c5ca-4f7d-a8f3-9b378bfc2886/regattaresult/494145d6-6ac8-42a9-adb8-a6824218e05f</t>
+  </si>
+  <si>
+    <t>Internacional. Laser-Kuhschellenregatta 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/d98c5acb-1157-4141-a459-ade8977620b0/regattaresult/49093fb6-a0c8-4005-9d78-25c2a21cd49c</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/d98c5acb-1157-4141-a459-ade8977620b0/regattaresult/7d7a9867-5636-4379-aacb-c4189776d2c0</t>
+  </si>
+  <si>
+    <t>EurILCA Campeonato Europeu Sub 21 e Troféu Europeu Aberto 2023</t>
+  </si>
+  <si>
+    <t>EurILCA Campeonato Europeu Sub 21 e Troféu Europeu Aberto</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/e5eb6cb9-f71a-4326-9640-7ba859eb4df2/regattaresult/eb19f998-5abb-4350-b6e5-f19d23a90085</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/e5eb6cb9-f71a-4326-9640-7ba859eb4df2/regattaresult/c60415f9-44d2-4fe2-9f24-f7400f12352b</t>
+  </si>
+  <si>
+    <t>Latvijas atklātais čempionāts 2023 Optimist e ILCA klasēm</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/18852d68-82f7-44af-8948-70ae9480bf54/regattaresult/e4969b8f-770d-4c8e-b308-b4663f1f009b</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/18852d68-82f7-44af-8948-70ae9480bf54/regattaresult/b9c8ccdc-53ca-485c-8115-4b3ee029531a</t>
+  </si>
+  <si>
+    <t>ILCANC 3  2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/b5097c69-91ec-4823-94fe-2022bf1505ac/regattaresult/dcc7455a-a052-4145-9a60-527e40e714a2</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/b5097c69-91ec-4823-94fe-2022bf1505ac/regattaresult/b23623ff-b4f4-4ec3-b21c-c719c71f58e0</t>
+  </si>
+  <si>
+    <t>Copa Surendorf 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/97dcda45-f887-4c1e-81e8-df819c2fda07/regattaresult/195c6974-ce8f-4e2d-976c-57e75a83c29c</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/97dcda45-f887-4c1e-81e8-df819c2fda07/regattaresult/46b705f1-deff-48ad-ac9f-c5df36c08d1c</t>
+  </si>
+  <si>
+    <t>Spandauer Eis-Cup 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/83f37faf-c4d2-41ba-8f96-529a9f56d778/regattaresult/381bdce2-abab-41d3-b531-0c6737a35252</t>
+  </si>
+  <si>
+    <t>LYC Youth Cup 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/8c39392b-6d6c-48e9-b686-23e651624e46/regattaresult/d19acdeb-4239-4cba-a13b-7f3b8605da98</t>
+  </si>
+  <si>
+    <t>DER WIKINGER 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/229a85ba-c23e-4257-bbba-b4af879062ae/regattaresult/ab2abd0f-b1fe-4102-9849-b4212d5b993d</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/229a85ba-c23e-4257-bbba-b4af879062ae/regattaresult/3dc707e9-c5cd-41b0-8bfd-e7d45634007b</t>
+  </si>
+  <si>
+    <t>ILCA6 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/ed99a262-7b97-4f79-89b8-326e3fd05e68/regattaresult/cd0a69ce-f468-462f-b4db-a43da09eafc2</t>
+  </si>
+  <si>
+    <t>ILCA7 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/82382487-1fcc-46bc-9ff9-5fc05c1b2e07/regattaresult/7de9b34e-53e7-47cf-a0b0-c36246a00e30</t>
+  </si>
+  <si>
+    <t>Nationale wedstrijd 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/d1e2dc90-a4bd-4065-9edb-36391f72670f/regattaresult/ae2cc32f-cc74-44dc-ba0a-51d395065fdc</t>
+  </si>
+  <si>
+    <t>Martinsregata II ILCA 2023</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/db3e82e7-af65-46a0-b2af-0892e1cedcfc/regattaresult/68532871-30e3-4033-a440-33b442c08591</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/db3e82e7-af65-46a0-b2af-0892e1cedcfc/regattaresult/39f9b4aa-e6a2-4981-9804-e0ef094ae804</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/a8ce7ffd-fb2b-4add-9ec4-2f3bb7e0fa40/regattaresult/91f91403-1bcc-4ff5-b8ef-9b10ec19fb44</t>
+  </si>
+  <si>
+    <t>https://manage2sail.com/api/event/a8ce7ffd-fb2b-4add-9ec4-2f3bb7e0fa40/regattaresult/072ae1fe-1b34-4572-8336-962771e440f3</t>
+  </si>
+  <si>
+    <t>Auftaktregatta - 2024 - ILCA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -286,14 +460,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -324,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -348,11 +514,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,13 +1233,13 @@
       <c r="A27" s="7">
         <v>470</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C27" s="2">
         <v>33</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1087,38 +1250,38 @@
       <c r="B28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="2">
         <v>34</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+      <c r="A29" s="7">
         <v>470</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="2">
         <v>35</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C30" s="2">
         <v>36</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1132,7 +1295,7 @@
       <c r="C31" s="2">
         <v>36</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1146,7 +1309,7 @@
       <c r="C32" s="2">
         <v>37</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1160,7 +1323,7 @@
       <c r="C33" s="2">
         <v>38</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1174,7 +1337,7 @@
       <c r="C34" s="2">
         <v>39</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1188,7 +1351,7 @@
       <c r="C35" s="2">
         <v>40</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1202,7 +1365,7 @@
       <c r="C36" s="2">
         <v>41</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1230,7 +1393,7 @@
       <c r="C38" s="2">
         <v>43</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1242,49 +1405,49 @@
         <v>72</v>
       </c>
       <c r="C39" s="2">
-        <v>44</v>
-      </c>
-      <c r="D39" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C40" s="2">
-        <v>45</v>
-      </c>
-      <c r="D40" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C41" s="2">
-        <v>45</v>
-      </c>
-      <c r="D41" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C42" s="2">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>80</v>
@@ -1292,17 +1455,496 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C43" s="2">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>79</v>
-      </c>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="2">
+        <v>50</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="2">
+        <v>50</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="2">
+        <v>51</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="2">
+        <v>51</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="2">
+        <v>52</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="2">
+        <v>54</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="2">
+        <v>55</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="2">
+        <v>55</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="2">
+        <v>56</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="2">
+        <v>57</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="2">
+        <v>58</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="2">
+        <v>59</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="2">
+        <v>60</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="2">
+        <v>61</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="2">
+        <v>61</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="2">
+        <v>59</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="2">
+        <v>60</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="2">
+        <v>62</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="2">
+        <v>62</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" s="2">
+        <v>64</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C64" s="2">
+        <v>63</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="2">
+        <v>64</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" s="2">
+        <v>65</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" s="2">
+        <v>65</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="2">
+        <v>66</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" s="2">
+        <v>67</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" s="2">
+        <v>67</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="2">
+        <v>68</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="2">
+        <v>69</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C73" s="2">
+        <v>70</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74" s="2">
+        <v>71</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" s="2">
+        <v>71</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" s="2">
+        <v>72</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" s="2">
+        <v>72</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D78" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
re add cluster 9 data
</commit_message>
<xml_diff>
--- a/scrapers/source-data/references.xlsx
+++ b/scrapers/source-data/references.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabmel\OneDrive\Documentos\fgv\field\-sailing-rankings-2024.1\scrapers\source-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silla\Desktop\Projetos\-sailing-rankings-2024.1\scrapers\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BF0727-67EE-43ED-9285-1E8F6ED361C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EAF686-2358-4458-BA49-AEB41787509C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
   <si>
     <t>Classe Vela</t>
   </si>
@@ -439,13 +439,25 @@
   </si>
   <si>
     <t>Auftaktregatta - ILCA 2024</t>
+  </si>
+  <si>
+    <t>World Championship 2019</t>
+  </si>
+  <si>
+    <t>https://www.manage2sail.com/api/event/0adf7bcd-01d0-4214-a295-bb0b9136999e/regattaresult/056dd04a-3fad-45f1-b9c2-894bdb176b43</t>
+  </si>
+  <si>
+    <t>https://www.manage2sail.com/api/event/41de110b-ec26-427d-81fb-be7807677326/regattaresult/5c147b15-f550-4046-ab46-203d9390ddb7</t>
+  </si>
+  <si>
+    <t>https://www.manage2sail.com/api/event/71c3d3a9-60fc-4465-816d-4b474c3ef34b/regattaresult/f9177157-d702-4601-b6d2-1a12e644a0fb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -466,16 +478,42 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -483,11 +521,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -510,8 +594,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -844,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1348,7 +1446,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>54</v>
       </c>
@@ -1460,7 +1558,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>72</v>
       </c>
@@ -1474,7 +1572,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>71</v>
       </c>
@@ -1488,7 +1586,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>72</v>
       </c>
@@ -1502,7 +1600,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -1544,7 +1642,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>72</v>
       </c>
@@ -1558,7 +1656,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>71</v>
       </c>
@@ -1614,7 +1712,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>72</v>
       </c>
@@ -1670,7 +1768,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
@@ -1684,7 +1782,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>71</v>
       </c>
@@ -1876,7 +1974,7 @@
       <c r="C73" s="2">
         <v>270</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="12" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1922,7 +2020,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>71</v>
       </c>
@@ -1936,16 +2034,69 @@
         <v>132</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D78"/>
+    <row r="78" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D24" r:id="rId1" display="https://manage2sail.com/api/event/c64b4c22-4afb-4889-9a4d-84ce7442aa35/regattaresult/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D25" r:id="rId2" display="https://manage2sail.com/api/event/c64b4c22-4afb-4889-9a4d-84ce7442aa35/regattaresult/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="D26" r:id="rId3" display="https://manage2sail.com/api/event/c64b4c22-4afb-4889-9a4d-84ce7442aa35/regattaresult/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D73" r:id="rId4" xr:uid="{D92C3F84-0915-430E-803B-533F45FF7628}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>